<commit_message>
Fixes employee ID and national ID display
Swapped the 'employee_id' and 'national_id' columns in the employee data import process to correct their display positions in the system, updating the `employee_template.xlsx` file and the `utils/excel.py` script's `parse_employee_excel` function to reflect the change.  Added error handling and improved column detection logic.  New template files (`employee_template_new.xlsx` and `employee_template_updated.xlsx`) were added.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 422fc151-3e5f-403a-a02c-9bf485bd995e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/d72f2aef-918c-4148-9723-15870f8c7cf6/7b6f3c71-7ed9-49fc-986f-9e20542a4279.jpg
</commit_message>
<xml_diff>
--- a/static/templates/employee_template.xlsx
+++ b/static/templates/employee_template.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Employees" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -27,24 +27,17 @@
     </font>
     <font>
       <b val="1"/>
-      <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00337AB7"/>
-        <bgColor rgb="00337AB7"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -52,17 +45,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,17 +432,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="8" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="9" customWidth="1" min="8" max="8"/>
-    <col width="23" customWidth="1" min="9" max="9"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -496,141 +481,141 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>موظف 1</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>EMP001</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>1234567890</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>0501234567</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>مدير</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>موظف الأول</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>N-5001001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>EMP1001</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0599123456</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>مدير قسم</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>نشط</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>الرياض</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>مشروع أ</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>مشروع التطوير</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>employee1@example.com</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>موظف 2</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>EMP002</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>2345678901</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>0512345678</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>محاسب</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>موظف الثاني</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>N-5002002</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>EMP1002</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0599234567</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>مهندس برمجيات</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>نشط</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>جدة</t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>مشروع ب</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>مشروع الدعم</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>employee2@example.com</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>موظف 3</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>EMP003</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>3456789012</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>0523456789</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>مهندس</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>on_leave</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>موظف الثالث</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>N-5003003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>EMP1003</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0599345678</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>محاسب</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>في إجازة</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>الدمام</t>
         </is>
       </c>
-      <c r="H4" s="2" t="inlineStr">
-        <is>
-          <t>مشروع ج</t>
-        </is>
-      </c>
-      <c r="I4" s="2" t="inlineStr">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>مشروع المالية</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>employee3@example.com</t>
         </is>

</xml_diff>